<commit_message>
state of the project
</commit_message>
<xml_diff>
--- a/20_Zeitplan/Zeitplanung_V2.xlsx
+++ b/20_Zeitplan/Zeitplanung_V2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b7schal\Documents\GitHub\GEM\20_Projektvereinbarung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b7schal\Documents\GitHub\GEM\20_Zeitplan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -199,7 +199,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -452,11 +452,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -492,10 +505,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -818,7 +830,7 @@
   <dimension ref="B5:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="I18" sqref="I18:J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1017,8 +1029,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="1"/>
+      <c r="I16" s="22"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1081,7 +1092,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="25"/>
       <c r="J20" s="25"/>
-      <c r="K20" s="1"/>
+      <c r="K20" s="36"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="15"/>
@@ -1095,8 +1106,8 @@
       <c r="F21" s="1"/>
       <c r="G21" s="33"/>
       <c r="I21" s="34"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="36"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="15"/>
@@ -1112,8 +1123,8 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="38"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="36"/>
       <c r="M22" s="1"/>
       <c r="N22" s="15"/>
     </row>
@@ -1174,7 +1185,7 @@
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B32" s="36"/>
+      <c r="B32" s="35"/>
       <c r="C32" t="s">
         <v>18</v>
       </c>

</xml_diff>